<commit_message>
Read file path fix
</commit_message>
<xml_diff>
--- a/lw3Tweets.xlsx
+++ b/lw3Tweets.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\tweet-fetcher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F8B052-731E-4237-B608-2FD677E58917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -45,20 +34,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,14 +369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.36328125" customWidth="1"/>
     <col min="2" max="2" width="10.36328125" customWidth="1"/>
@@ -396,7 +385,7 @@
     <col min="5" max="5" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" ht="26.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,6 +404,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>